<commit_message>
Poprawki w klocki.xlsx, funkcje Inicjalizuj, Rysuj, Pauza
</commit_message>
<xml_diff>
--- a/klocki.xlsx
+++ b/klocki.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INFORMATYKA UWR\C\TETRIS-Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64F5237-3170-4868-8D7F-CDC659ABBCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="4">
+  <si>
+    <t>ŚR</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>3 (1)</t>
+  </si>
+  <si>
+    <t>4 (2)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +52,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -45,15 +104,260 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +634,791 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="6.5546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="6.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="4"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="15"/>
+      <c r="W2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="4"/>
+    </row>
+    <row r="3" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="7"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="11"/>
+      <c r="W3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="7"/>
+    </row>
+    <row r="4" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5"/>
+      <c r="U4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="N5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V5" s="11"/>
+      <c r="W5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="7"/>
+    </row>
+    <row r="6" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="10"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9"/>
+      <c r="X6" s="10"/>
+    </row>
+    <row r="7" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
+      <c r="T8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="4"/>
+      <c r="T9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="20"/>
+      <c r="V9" s="4"/>
+    </row>
+    <row r="10" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="V10" s="18"/>
+      <c r="W10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="8"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="10"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="19"/>
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6">
+        <v>2</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6">
+        <v>3</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6">
+        <v>4</v>
+      </c>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="4"/>
+      <c r="X20" s="6"/>
+    </row>
+    <row r="21" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="24"/>
+      <c r="C21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="7"/>
+      <c r="X21" s="6"/>
+    </row>
+    <row r="22" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="43"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="46"/>
+      <c r="X22" s="6"/>
+    </row>
+    <row r="23" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+    </row>
+    <row r="25" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="N25" s="1">
+        <v>3</v>
+      </c>
+      <c r="T25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="4"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="4"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="55"/>
+    </row>
+    <row r="27" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="47"/>
+      <c r="C27" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="49"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="V27" s="7"/>
+    </row>
+    <row r="28" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="50"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="10"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="10"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="10"/>
+    </row>
+    <row r="32" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="2"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="28"/>
+      <c r="J33" s="4"/>
+      <c r="M33"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U33" s="28"/>
+      <c r="V33" s="4"/>
+    </row>
+    <row r="34" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="H34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="30"/>
+      <c r="K34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M34" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="N34" s="26"/>
+      <c r="O34" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P34" s="7"/>
+      <c r="Q34"/>
+      <c r="T34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U34" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="V34" s="30"/>
+      <c r="W34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35"/>
+      <c r="N35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P35" s="10"/>
+      <c r="Q35"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="V36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="4"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="34"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="4"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="37"/>
+      <c r="W38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="5"/>
+      <c r="C39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="33"/>
+      <c r="E39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33"/>
+      <c r="K39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="5"/>
+      <c r="O39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T39" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="V39" s="33"/>
+      <c r="W39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="8"/>
+      <c r="C40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="36"/>
+      <c r="J40" s="10"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T40" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U40" s="36"/>
+      <c r="V40" s="10"/>
+    </row>
+    <row r="41" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
obrot.txt, dodanie obrotu do klocki.xlsx, przykladowe funkcje Lewo, Prawo, Dol dla T
</commit_message>
<xml_diff>
--- a/klocki.xlsx
+++ b/klocki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INFORMATYKA UWR\C\TETRIS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64F5237-3170-4868-8D7F-CDC659ABBCEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0842179-77AE-4E5B-B8EB-965224DEF46A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,25 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="2">
   <si>
     <t>ŚR</t>
   </si>
   <si>
     <t>x</t>
   </si>
-  <si>
-    <t>3 (1)</t>
-  </si>
-  <si>
-    <t>4 (2)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,8 +45,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +93,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,9 +332,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,6 +369,84 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="Z38" sqref="Z38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z42" sqref="Z42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -672,9 +766,9 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="4"/>
       <c r="T2" s="2"/>
@@ -682,15 +776,15 @@
         <v>1</v>
       </c>
       <c r="V2" s="15"/>
-      <c r="W2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="4"/>
+      <c r="W2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="63"/>
     </row>
     <row r="3" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="H3" s="5"/>
@@ -698,13 +792,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="55" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="7"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="7"/>
       <c r="T3" s="5"/>
@@ -712,10 +806,10 @@
         <v>1</v>
       </c>
       <c r="V3" s="11"/>
-      <c r="W3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="7"/>
+      <c r="W3" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="56"/>
     </row>
     <row r="4" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -730,14 +824,14 @@
       <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="55" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="55" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="7"/>
@@ -754,33 +848,33 @@
         <v>1</v>
       </c>
       <c r="T4" s="5"/>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="55" t="s">
         <v>1</v>
       </c>
       <c r="V4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X4" s="7"/>
+      <c r="W4" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" s="56"/>
     </row>
     <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6" t="s">
+      <c r="D5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="59"/>
+      <c r="I5" s="55" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="11"/>
@@ -794,15 +888,15 @@
       <c r="O5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="P5" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="55" t="s">
         <v>1</v>
       </c>
       <c r="R5" s="7"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="55" t="s">
         <v>1</v>
       </c>
       <c r="V5" s="11"/>
@@ -814,11 +908,11 @@
     <row r="6" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9" t="s">
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="57" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="13"/>
@@ -859,22 +953,26 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="4"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="I9" s="20"/>
-      <c r="J9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2"/>
+      <c r="J9" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="61"/>
       <c r="O9" s="20"/>
-      <c r="P9" s="4"/>
+      <c r="P9" s="63"/>
       <c r="T9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="U9" s="20"/>
-      <c r="V9" s="4"/>
+      <c r="V9" s="63" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -895,7 +993,7 @@
       <c r="I10" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="56" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -909,7 +1007,7 @@
       <c r="Q10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="T10" s="59" t="s">
         <v>1</v>
       </c>
       <c r="U10" s="17" t="s">
@@ -921,10 +1019,16 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="8"/>
+      <c r="B11" s="60" t="s">
+        <v>1</v>
+      </c>
       <c r="C11" s="19"/>
-      <c r="D11" s="10"/>
-      <c r="H11" s="8"/>
+      <c r="D11" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>1</v>
+      </c>
       <c r="I11" s="19"/>
       <c r="J11" s="10" t="s">
         <v>1</v>
@@ -932,17 +1036,19 @@
       <c r="N11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T11" s="8" t="s">
+      <c r="O11" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="60" t="s">
         <v>1</v>
       </c>
       <c r="U11" s="19"/>
-      <c r="V11" s="10"/>
+      <c r="V11" s="58" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
@@ -980,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -988,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>1</v>
       </c>
@@ -1019,91 +1125,144 @@
       <c r="V19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+    <row r="20" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
       <c r="D20" s="4"/>
       <c r="E20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="44"/>
+      <c r="G20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="43"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="4"/>
+      <c r="J20" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="6"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="2"/>
+      <c r="T20" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="U20" s="25"/>
-      <c r="V20" s="4"/>
+      <c r="V20" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="B21" s="24"/>
       <c r="C21" s="21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="22"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="59" t="s">
+        <v>1</v>
+      </c>
       <c r="I21" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="J21" s="7"/>
+      <c r="J21" s="56" t="s">
+        <v>1</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="N21" s="24"/>
       <c r="O21" s="21" t="s">
         <v>0</v>
       </c>
       <c r="P21" s="22"/>
-      <c r="Q21" s="6"/>
+      <c r="Q21" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
-      <c r="T21" s="5"/>
+      <c r="T21" s="59" t="s">
+        <v>1</v>
+      </c>
       <c r="U21" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="V21" s="7"/>
+      <c r="V21" s="56" t="s">
+        <v>1</v>
+      </c>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="43"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
+    <row r="22" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>1</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="8"/>
+      <c r="H22" s="60" t="s">
+        <v>1</v>
+      </c>
       <c r="I22" s="23"/>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="10"/>
+      <c r="N22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="58" t="s">
+        <v>1</v>
+      </c>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
-      <c r="T22" s="8"/>
+      <c r="T22" s="60" t="s">
+        <v>1</v>
+      </c>
       <c r="U22" s="23"/>
-      <c r="V22" s="46"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
+    <row r="23" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -1115,12 +1274,16 @@
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
+      <c r="U23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="25" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
         <v>1</v>
       </c>
@@ -1134,72 +1297,144 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
+    <row r="26" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="4"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="4"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="4"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="55"/>
-    </row>
-    <row r="27" spans="2:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="47"/>
-      <c r="C27" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="49"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="J27" s="7"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="P27" s="49"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="V27" s="7"/>
-    </row>
-    <row r="28" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="50"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="10"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="10"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="10"/>
-    </row>
-    <row r="32" spans="2:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="50"/>
+      <c r="J26" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="53"/>
+      <c r="O26" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="P26" s="63"/>
+      <c r="T26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U26" s="50"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="46"/>
+      <c r="O27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T27" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="U27" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="V27" s="56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="E28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T28" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="51"/>
+      <c r="V28" s="58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="H32" s="1">
         <v>2</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T32" s="1" t="s">
+      <c r="N32" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="T32" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
       <c r="E33" s="1" t="s">
@@ -1209,21 +1444,22 @@
         <v>1</v>
       </c>
       <c r="I33" s="28"/>
-      <c r="J33" s="4"/>
-      <c r="M33"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" t="s">
-        <v>1</v>
-      </c>
-      <c r="T33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U33" s="28"/>
-      <c r="V33" s="4"/>
-    </row>
-    <row r="34" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" s="68"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="4"/>
+      <c r="S33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" s="66"/>
+      <c r="U33" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="V33" s="72"/>
+    </row>
+    <row r="34" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1231,7 +1467,9 @@
       <c r="C34" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="56" t="s">
+        <v>1</v>
+      </c>
       <c r="H34" s="5" t="s">
         <v>1</v>
       </c>
@@ -1242,111 +1480,117 @@
       <c r="K34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M34" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="N34" s="26"/>
+      <c r="N34" s="69" t="s">
+        <v>1</v>
+      </c>
       <c r="O34" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="P34" s="7"/>
-      <c r="Q34"/>
-      <c r="T34" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T34" s="26"/>
       <c r="U34" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="V34" s="30"/>
-      <c r="W34" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V34" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="9"/>
+      <c r="D35" s="58"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="57" t="s">
+        <v>1</v>
+      </c>
       <c r="J35" s="31"/>
       <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M35"/>
-      <c r="N35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P35" s="10"/>
-      <c r="Q35"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="31"/>
-      <c r="W35" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35" s="64"/>
+      <c r="O35" s="65"/>
+      <c r="P35" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="T35" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="U35" s="65"/>
+      <c r="V35" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="V36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1">
         <v>1</v>
       </c>
       <c r="H37" s="1">
         <v>2</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T37" s="1" t="s">
+      <c r="N37" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T37" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="34"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="72" t="s">
+        <v>1</v>
+      </c>
       <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="J38" s="37"/>
       <c r="K38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N38" s="34"/>
-      <c r="O38" s="35"/>
+      <c r="N38" s="68"/>
+      <c r="O38" s="71"/>
       <c r="P38" s="4"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="37"/>
-      <c r="W38" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="5"/>
+      <c r="T38" s="68"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="C39" s="32" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1598,7 @@
       <c r="E39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H39" s="69" t="s">
         <v>1</v>
       </c>
       <c r="I39" s="32" t="s">
@@ -1364,56 +1608,70 @@
       <c r="K39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="5"/>
+      <c r="M39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="75"/>
       <c r="O39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T39" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="P39" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T39" s="75"/>
       <c r="U39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="V39" s="33"/>
-      <c r="W39" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V39" s="79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="8"/>
-      <c r="C40" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="8" t="s">
+      <c r="C40" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="70" t="s">
         <v>1</v>
       </c>
       <c r="I40" s="36"/>
-      <c r="J40" s="10"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T40" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U40" s="36"/>
+      <c r="J40" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="N40" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="O40" s="73"/>
+      <c r="P40" s="74"/>
+      <c r="Q40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T40" s="76"/>
+      <c r="U40" s="80" t="s">
+        <v>1</v>
+      </c>
       <c r="V40" s="10"/>
     </row>
-    <row r="41" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U41" s="1" t="s">
+      <c r="O41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
struct Klocek, schematy 7 klockow, funkcja Spadek z losowaniem nowego klocka
</commit_message>
<xml_diff>
--- a/klocki.xlsx
+++ b/klocki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INFORMATYKA UWR\C\TETRIS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0842179-77AE-4E5B-B8EB-965224DEF46A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0633379-37EF-4CFE-97A4-CC64895A4282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -732,7 +732,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z42" sqref="Z42"/>
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1417,137 +1417,137 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1">
+    <row r="31" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
         <v>2</v>
       </c>
-      <c r="N32" s="1">
+      <c r="N31" s="1">
         <v>3</v>
       </c>
-      <c r="T32" s="1">
+      <c r="T31" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
+    <row r="32" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="68"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="G32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="66"/>
+      <c r="I32" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" s="72"/>
+      <c r="N32" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="O32" s="28"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U32" s="28"/>
+      <c r="V32" s="63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="30"/>
       <c r="E33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="N33" s="68"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="4"/>
-      <c r="S33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T33" s="66"/>
-      <c r="U33" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="V33" s="72"/>
-    </row>
-    <row r="34" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="26"/>
+      <c r="I33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" s="26"/>
+      <c r="O33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P33" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U33" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="V33" s="30"/>
+      <c r="W33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J34" s="30"/>
-      <c r="K34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N34" s="69" t="s">
-        <v>1</v>
-      </c>
-      <c r="O34" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T34" s="26"/>
-      <c r="U34" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="58"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="J35" s="31"/>
-      <c r="K35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N35" s="64"/>
-      <c r="O35" s="65"/>
-      <c r="P35" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="T35" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="U35" s="65"/>
-      <c r="V35" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="64"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="65"/>
+      <c r="J34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P34" s="58"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="V34" s="31"/>
+      <c r="W34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1">
         <v>1</v>
       </c>
@@ -1561,117 +1561,117 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J38" s="37"/>
-      <c r="K38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N38" s="68"/>
-      <c r="O38" s="71"/>
-      <c r="P38" s="4"/>
-      <c r="T38" s="68"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="72" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="5" t="s">
-        <v>1</v>
-      </c>
+    <row r="38" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="68"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="4"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N38" s="34"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="T38" s="2"/>
+      <c r="U38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V38" s="37"/>
+      <c r="W38" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="75"/>
       <c r="C39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="33"/>
-      <c r="E39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39" s="69" t="s">
-        <v>1</v>
-      </c>
+      <c r="D39" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="75"/>
       <c r="I39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J39" s="33"/>
-      <c r="K39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N39" s="75"/>
+      <c r="J39" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="O39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="P39" s="78" t="s">
-        <v>1</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T39" s="75"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T39" s="69" t="s">
+        <v>1</v>
+      </c>
       <c r="U39" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="V39" s="79" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="8"/>
-      <c r="C40" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="I40" s="36"/>
-      <c r="J40" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="N40" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="O40" s="73"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T40" s="76"/>
-      <c r="U40" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="V40" s="10"/>
-    </row>
-    <row r="41" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T41" s="1" t="s">
+      <c r="V39" s="33"/>
+      <c r="W39" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="73"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="76"/>
+      <c r="I40" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="P40" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="T40" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="U40" s="36"/>
+      <c r="V40" s="67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U41" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dodanie siatki do Klockow, zmieniony rozmiar planszy, funkcja Obrot (ale znow zle dziala)
</commit_message>
<xml_diff>
--- a/klocki.xlsx
+++ b/klocki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INFORMATYKA UWR\C\TETRIS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0633379-37EF-4CFE-97A4-CC64895A4282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB1C17A-CB2A-4E9D-A21F-44D713390023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12576" yWindow="168" windowWidth="13308" windowHeight="11508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="52">
   <si>
     <t>ŚR</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>0 0</t>
+  </si>
+  <si>
+    <t>1 0</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>2 0</t>
+  </si>
+  <si>
+    <t>3 0</t>
+  </si>
+  <si>
+    <t>4 0</t>
+  </si>
+  <si>
+    <t>0 1</t>
+  </si>
+  <si>
+    <t>2 1</t>
+  </si>
+  <si>
+    <t>3 1</t>
+  </si>
+  <si>
+    <t>4 1</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>1 2</t>
+  </si>
+  <si>
+    <t>2 2</t>
+  </si>
+  <si>
+    <t>3 2</t>
+  </si>
+  <si>
+    <t>4 2</t>
+  </si>
+  <si>
+    <t>0 3</t>
+  </si>
+  <si>
+    <t>1 3</t>
+  </si>
+  <si>
+    <t>2 3</t>
+  </si>
+  <si>
+    <t>3 3</t>
+  </si>
+  <si>
+    <t>4 3</t>
+  </si>
+  <si>
+    <t>0 4</t>
+  </si>
+  <si>
+    <t>1 4</t>
+  </si>
+  <si>
+    <t>2 4</t>
+  </si>
+  <si>
+    <t>3 4</t>
+  </si>
+  <si>
+    <t>4 4</t>
+  </si>
+  <si>
+    <t>4 5</t>
+  </si>
+  <si>
+    <t>5 5</t>
+  </si>
+  <si>
+    <t>6 5</t>
+  </si>
+  <si>
+    <t>7 5</t>
+  </si>
+  <si>
+    <t>8 5</t>
+  </si>
+  <si>
+    <t>4 6</t>
+  </si>
+  <si>
+    <t>5 6</t>
+  </si>
+  <si>
+    <t>6 6</t>
+  </si>
+  <si>
+    <t>7 6</t>
+  </si>
+  <si>
+    <t>8 6</t>
+  </si>
+  <si>
+    <t>4 7</t>
+  </si>
+  <si>
+    <t>5 7</t>
+  </si>
+  <si>
+    <t>6 7</t>
+  </si>
+  <si>
+    <t>7 7</t>
+  </si>
+  <si>
+    <t>8 7</t>
+  </si>
+  <si>
+    <t>4 8</t>
+  </si>
+  <si>
+    <t>5 8</t>
+  </si>
+  <si>
+    <t>6 8</t>
+  </si>
+  <si>
+    <t>8 8</t>
+  </si>
+  <si>
+    <t>7 8</t>
+  </si>
+  <si>
+    <t>4 9</t>
+  </si>
+  <si>
+    <t>5 9</t>
+  </si>
+  <si>
+    <t>6 9</t>
+  </si>
+  <si>
+    <t>7 9</t>
+  </si>
+  <si>
+    <t>8 9</t>
   </si>
 </sst>
 </file>
@@ -731,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1059,21 +1209,115 @@
       </c>
       <c r="U12" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>1</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="38" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" s="39"/>
       <c r="D15" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1085,13 +1329,73 @@
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" s="56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="P17" s="58" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Aktualizacja klocki.xlsx, wyswietlanie komunikatu o high score
</commit_message>
<xml_diff>
--- a/klocki.xlsx
+++ b/klocki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\INFORMATYKA UWR\C\TETRIS-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A8F2BE-CE66-41FF-823E-0B0195440CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86F6E58-A368-481C-A63B-A1D9904046E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7068" yWindow="7656" windowWidth="13308" windowHeight="11508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="56">
   <si>
     <t>ŚR</t>
   </si>
@@ -183,22 +183,16 @@
     <t>8 9</t>
   </si>
   <si>
-    <t>6 3</t>
-  </si>
-  <si>
-    <t>5 3</t>
-  </si>
-  <si>
-    <t>7 3</t>
-  </si>
-  <si>
-    <t>5 4</t>
-  </si>
-  <si>
-    <t>6 4</t>
-  </si>
-  <si>
-    <t>7 4</t>
+    <t>zakazane</t>
+  </si>
+  <si>
+    <t>punkty do sprawdzenia</t>
+  </si>
+  <si>
+    <t>w Lewo, Prawo, Dol</t>
+  </si>
+  <si>
+    <t>Siatka</t>
   </si>
 </sst>
 </file>
@@ -375,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -615,6 +609,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -897,19 +918,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="6.5546875" style="1"/>
+    <col min="2" max="26" width="6.5546875" style="1"/>
+    <col min="27" max="27" width="20.44140625" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="6.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -923,7 +946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -934,8 +957,8 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="62"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
       <c r="P2" s="62"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="4"/>
@@ -944,14 +967,18 @@
         <v>1</v>
       </c>
       <c r="V2" s="15"/>
-      <c r="W2" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="63"/>
-    </row>
-    <row r="3" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W2" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="87"/>
+      <c r="Z2" s="88"/>
+      <c r="AA2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5"/>
-      <c r="C3" s="55"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="55"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
@@ -960,12 +987,12 @@
         <v>1</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="82" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="7"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="55"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="82"/>
       <c r="P3" s="55"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="7"/>
@@ -974,12 +1001,18 @@
         <v>1</v>
       </c>
       <c r="V3" s="11"/>
-      <c r="W3" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="56"/>
-    </row>
-    <row r="4" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="78"/>
+      <c r="Z3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1026,8 +1059,11 @@
         <v>1</v>
       </c>
       <c r="X4" s="56"/>
-    </row>
-    <row r="5" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>1</v>
@@ -1035,14 +1071,14 @@
       <c r="D5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="59"/>
-      <c r="I5" s="55" t="s">
+      <c r="E5" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="81"/>
+      <c r="I5" s="82" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="11"/>
@@ -1059,12 +1095,12 @@
       <c r="P5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="Q5" s="55" t="s">
+      <c r="Q5" s="82" t="s">
         <v>1</v>
       </c>
       <c r="R5" s="7"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="55" t="s">
+      <c r="U5" s="82" t="s">
         <v>1</v>
       </c>
       <c r="V5" s="11"/>
@@ -1073,14 +1109,14 @@
       </c>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="57" t="s">
+      <c r="E6" s="80"/>
+      <c r="F6" s="84"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="80" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="13"/>
@@ -1101,12 +1137,12 @@
       <c r="W6" s="9"/>
       <c r="X6" s="10"/>
     </row>
-    <row r="7" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -1120,29 +1156,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61"/>
+    <row r="9" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="85"/>
       <c r="C9" s="62"/>
       <c r="D9" s="4"/>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="85" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="20"/>
-      <c r="J9" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="61"/>
+      <c r="J9" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="85"/>
       <c r="O9" s="20"/>
-      <c r="P9" s="63"/>
+      <c r="P9" s="87"/>
       <c r="T9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="U9" s="20"/>
-      <c r="V9" s="63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1186,15 +1222,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="60" t="s">
+    <row r="11" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="83" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="19"/>
-      <c r="D11" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="60" t="s">
+      <c r="D11" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="83" t="s">
         <v>1</v>
       </c>
       <c r="I11" s="19"/>
@@ -1207,18 +1243,18 @@
       <c r="O11" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="P11" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T11" s="60" t="s">
+      <c r="P11" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="83" t="s">
         <v>1</v>
       </c>
       <c r="U11" s="19"/>
-      <c r="V11" s="58" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V11" s="84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1229,92 +1265,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="N14" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="R14" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="V14" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="W14" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="X14" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1325,56 +1281,8 @@
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="S15" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="V15" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="W15" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="X15" s="58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:27" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1383,91 +1291,13 @@
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="55" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="N16" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="O16" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="P16" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="R16" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="S16" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="T16" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="V16" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="W16" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="X16" s="58" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N17" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="P17" s="58" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1517,7 +1347,7 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="61"/>
+      <c r="N20" s="85"/>
       <c r="O20" s="62"/>
       <c r="P20" s="44"/>
       <c r="Q20" s="6" t="s">
@@ -1529,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="25"/>
-      <c r="V20" s="63" t="s">
+      <c r="V20" s="87" t="s">
         <v>1</v>
       </c>
       <c r="X20" s="6"/>
@@ -1590,12 +1420,12 @@
       <c r="C22" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="84" t="s">
         <v>1</v>
       </c>
       <c r="E22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="60" t="s">
+      <c r="H22" s="83" t="s">
         <v>1</v>
       </c>
       <c r="I22" s="23"/>
@@ -1674,14 +1504,14 @@
       </c>
     </row>
     <row r="26" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="62"/>
       <c r="D26" s="4"/>
       <c r="H26" s="61" t="s">
         <v>1</v>
       </c>
       <c r="I26" s="50"/>
-      <c r="J26" s="63" t="s">
+      <c r="J26" s="87" t="s">
         <v>1</v>
       </c>
       <c r="M26" s="1" t="s">
@@ -1768,10 +1598,10 @@
       <c r="O28" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="P28" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T28" s="60" t="s">
+      <c r="P28" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="T28" s="83" t="s">
         <v>1</v>
       </c>
       <c r="U28" s="51"/>
@@ -1819,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="J32" s="72"/>
-      <c r="N32" s="61" t="s">
+      <c r="N32" s="85" t="s">
         <v>1</v>
       </c>
       <c r="O32" s="28"/>
@@ -1831,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="U32" s="28"/>
-      <c r="V32" s="63" t="s">
+      <c r="V32" s="87" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1883,10 +1713,10 @@
       </c>
       <c r="B34" s="64"/>
       <c r="C34" s="65"/>
-      <c r="D34" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="70" t="s">
+      <c r="D34" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="83" t="s">
         <v>1</v>
       </c>
       <c r="I34" s="65"/>
@@ -1938,12 +1768,12 @@
       </c>
     </row>
     <row r="38" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="68"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="71"/>
       <c r="D38" s="4"/>
       <c r="H38" s="68"/>
       <c r="I38" s="35"/>
-      <c r="J38" s="72" t="s">
+      <c r="J38" s="87" t="s">
         <v>1</v>
       </c>
       <c r="M38" s="1" t="s">
@@ -2026,10 +1856,10 @@
       <c r="O40" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="P40" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="T40" s="70" t="s">
+      <c r="P40" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="T40" s="83" t="s">
         <v>1</v>
       </c>
       <c r="U40" s="36"/>
@@ -2051,7 +1881,198 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+    </row>
+    <row r="44" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I45" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+    </row>
+    <row r="46" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K46" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+    </row>
+    <row r="47" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="L47" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+    </row>
+    <row r="48" spans="1:23" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J48" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="K48" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="L48" s="58" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B43:D43"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>